<commit_message>
Date based news & Excuting in a certain hour
</commit_message>
<xml_diff>
--- a/App-7-Automated-Emails/people.xlsx
+++ b/App-7-Automated-Emails/people.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mido Hany\VS code Projects\Python\Advanced_OOP\App-7-Automated-Emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89613312-3FC1-46D4-885F-526C5527C80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE43ED25-3F2A-488A-BFA2-A2C72B405216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,41 +34,46 @@
     <t>Soso</t>
   </si>
   <si>
+    <t>jajon28656@anwarb.com</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
     <t>Lolo</t>
   </si>
   <si>
-    <t>Football</t>
+    <t>Messi</t>
   </si>
   <si>
     <t>Toto</t>
   </si>
   <si>
-    <t>pawefibe@afia.pro</t>
-  </si>
-  <si>
-    <t>ezana.zethan@donebyngle.com</t>
-  </si>
-  <si>
-    <t>Messi</t>
+    <t>sxdp3fpkzql@ezztt.com</t>
   </si>
   <si>
     <t>Mojo</t>
   </si>
   <si>
-    <t>jajon28656@anwarb.com</t>
+    <t>hans.che@donebyngle.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -87,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,14 +100,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,62 +429,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{DF90C901-42C2-4D89-A2AE-375B88F1E0F1}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{82F9D50B-DBE4-403B-8A9E-00336FABBEED}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>